<commit_message>
new results, tables, graphs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>jezebel</t>
   </si>
@@ -64,12 +64,42 @@
   </si>
   <si>
     <t>K20 keff</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>usd</t>
+  </si>
+  <si>
+    <t>watt</t>
+  </si>
+  <si>
+    <t>cpu</t>
+  </si>
+  <si>
+    <t>watts</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>nps</t>
+  </si>
+  <si>
+    <t>total cycles</t>
+  </si>
+  <si>
+    <t>titan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -112,7 +142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -126,23 +156,161 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,79 +640,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:F32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>1.0000500000000001</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
+        <v>7.7000000000000001E-5</v>
+      </c>
+      <c r="D2">
         <v>0.99995000000000001</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="F2">
         <v>0.99977099999999997</v>
       </c>
-      <c r="E2">
-        <f>(D2-B2)*100000</f>
+      <c r="G2" s="1">
+        <v>9.5759831300000004E-5</v>
+      </c>
+      <c r="H2">
+        <f>(F2-B2)*100000</f>
         <v>-27.900000000014025</v>
       </c>
-      <c r="F2">
-        <f>(D2-C2)*100000</f>
+      <c r="I2">
+        <f>(F2-D2)*100000</f>
         <v>-17.900000000004024</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>0.59338500000000005</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
+        <v>9.7999999999999997E-5</v>
+      </c>
+      <c r="D3">
         <v>0.59272999999999998</v>
       </c>
-      <c r="D3">
+      <c r="E3">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F3">
         <v>0.59229500000000002</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E7" si="0">(D3-B3)*100000</f>
+      <c r="G3" s="1">
+        <v>9.5759831300000004E-5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="0">(F3-B3)*100000</f>
         <v>-109.00000000000354</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F7" si="1">(D3-C3)*100000</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I7" si="1">(F3-D3)*100000</f>
         <v>-43.499999999996319</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -552,164 +747,263 @@
         <v>0.27540100000000001</v>
       </c>
       <c r="C4">
+        <v>4.4999999999999999E-4</v>
+      </c>
+      <c r="D4">
         <v>0.27517000000000003</v>
       </c>
-      <c r="D4">
+      <c r="E4">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F4">
         <v>0.27410600000000002</v>
       </c>
-      <c r="E4">
+      <c r="G4" s="1">
+        <v>9.5759831300000004E-5</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>-129.49999999999906</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <f t="shared" si="1"/>
         <v>-106.40000000000094</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>0.88048999999999999</v>
       </c>
+      <c r="C5" s="1">
+        <v>6.9999999999999994E-5</v>
+      </c>
       <c r="D5">
+        <v>0.88085999999999998</v>
+      </c>
+      <c r="E5">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="F5">
         <v>0.87570099999999995</v>
       </c>
-      <c r="E5">
+      <c r="G5" s="1">
+        <v>9.5759831300000004E-5</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>-478.9000000000043</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <f t="shared" si="1"/>
-        <v>87570.099999999991</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>-515.90000000000248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>1.0986800000000001</v>
       </c>
+      <c r="C6" s="1">
+        <v>6.3999999999999997E-5</v>
+      </c>
       <c r="D6">
+        <v>1.1009899999999999</v>
+      </c>
+      <c r="E6">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="F6">
         <v>1.096884</v>
       </c>
-      <c r="E6">
+      <c r="G6" s="1">
+        <v>9.5759831300000004E-5</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>-179.6000000000131</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <f t="shared" si="1"/>
-        <v>109688.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>-410.59999999999428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>1.0757000000000001</v>
       </c>
+      <c r="C7" s="1">
+        <v>6.2000000000000003E-5</v>
+      </c>
       <c r="D7">
+        <v>0.88634000000000002</v>
+      </c>
+      <c r="E7">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="F7">
         <v>1.0740259999999999</v>
       </c>
-      <c r="E7">
+      <c r="G7" s="1">
+        <v>7.8187578799999996E-5</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>-167.40000000001754</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <f t="shared" si="1"/>
-        <v>107402.59999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>18768.599999999991</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10">
         <v>10.34</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>37.200000000000003</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E10">
-        <f>B10/D10</f>
+      <c r="H10">
+        <f t="shared" ref="H10:H15" si="2">B10/F10</f>
         <v>2.2478260869565219</v>
       </c>
-      <c r="F10">
-        <f>C10/D10</f>
+      <c r="I10">
+        <f>D10/F10</f>
         <v>8.0869565217391308</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="J10">
+        <v>60</v>
+      </c>
+      <c r="K10" s="1">
+        <v>9500000</v>
+      </c>
+      <c r="L10" s="2">
+        <f>J10*K10/(B10*60)</f>
+        <v>918762.08897485491</v>
+      </c>
+      <c r="M10" s="2">
+        <f>J10*K10/(60*D10)</f>
+        <v>255376.34408602151</v>
+      </c>
+      <c r="N10" s="2">
+        <f>J10*K10/(60*F10)</f>
+        <v>2065217.3913043479</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11">
         <v>57.84</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>133.37</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>10.93</v>
       </c>
-      <c r="E11">
-        <f t="shared" ref="E11:F15" si="2">B11/D11</f>
+      <c r="H11">
+        <f t="shared" si="2"/>
         <v>5.2918572735590121</v>
       </c>
-      <c r="F11">
-        <f t="shared" ref="F11:F15" si="3">C11/D11</f>
+      <c r="I11">
+        <f t="shared" ref="I11:I15" si="3">D11/F11</f>
         <v>12.202195791399818</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="J11">
+        <v>60</v>
+      </c>
+      <c r="K11" s="1">
+        <v>9500000</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" ref="L11:N15" si="4">J11*K11/(B11*60)</f>
+        <v>164246.19640387275</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" ref="M11:M15" si="5">J11*K11/(60*D11)</f>
+        <v>71230.411636799879</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" ref="N11:N15" si="6">J11*K11/(60*F11)</f>
+        <v>869167.42909423611</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12">
         <v>198.57</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>177.38</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>30.43</v>
       </c>
-      <c r="E12">
+      <c r="H12">
         <f t="shared" si="2"/>
         <v>6.5254682878738084</v>
       </c>
-      <c r="F12">
+      <c r="I12">
         <f t="shared" si="3"/>
         <v>5.8291160039434766</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="J12">
+        <v>60</v>
+      </c>
+      <c r="K12" s="1">
+        <v>9500000</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="4"/>
+        <v>47842.070806264797</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="5"/>
+        <v>53557.334536024355</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="6"/>
+        <v>312191.91587249428</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -717,18 +1011,39 @@
         <v>114.65</v>
       </c>
       <c r="D13">
+        <v>416.76666666666603</v>
+      </c>
+      <c r="F13">
         <v>31.99</v>
       </c>
-      <c r="E13">
+      <c r="H13">
         <f t="shared" si="2"/>
         <v>3.5839324788996567</v>
       </c>
-      <c r="F13">
+      <c r="I13">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>13.028029592580996</v>
+      </c>
+      <c r="J13">
+        <v>60</v>
+      </c>
+      <c r="K13" s="1">
+        <v>9500000</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="4"/>
+        <v>82860.880941997384</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="5"/>
+        <v>22794.529312964925</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="6"/>
+        <v>296967.80243826198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -736,18 +1051,39 @@
         <v>185.78</v>
       </c>
       <c r="D14">
+        <v>494.3</v>
+      </c>
+      <c r="F14">
         <v>73.73</v>
       </c>
-      <c r="E14">
+      <c r="H14">
         <f t="shared" si="2"/>
         <v>2.5197341651973417</v>
       </c>
-      <c r="F14">
+      <c r="I14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>6.7041909670419093</v>
+      </c>
+      <c r="J14">
+        <v>60</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8500000</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="4"/>
+        <v>45753.041231564217</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="5"/>
+        <v>17196.034796682176</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="6"/>
+        <v>115285.50115285501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -755,166 +1091,253 @@
         <v>122.43</v>
       </c>
       <c r="D15">
+        <v>316.45</v>
+      </c>
+      <c r="F15">
         <v>41.55</v>
       </c>
-      <c r="E15">
+      <c r="H15">
         <f t="shared" si="2"/>
         <v>2.9465703971119139</v>
       </c>
-      <c r="F15">
+      <c r="I15">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>7.6161251504211798</v>
+      </c>
+      <c r="J15">
+        <v>60</v>
+      </c>
+      <c r="K15" s="1">
+        <v>9500000</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="4"/>
+        <v>77595.360614228543</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="5"/>
+        <v>30020.540369726656</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="6"/>
+        <v>228640.1925391095</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="s">
+      <c r="H18" t="s">
         <v>9</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="B19">
         <v>9.9978400000000001</v>
       </c>
+      <c r="C19" s="1">
+        <v>9.5000000000000005E-5</v>
+      </c>
       <c r="D19">
+        <v>0.99982000000000004</v>
+      </c>
+      <c r="E19">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="F19">
         <v>0.99977099999999997</v>
       </c>
-      <c r="E19">
-        <f>(D19-B19)*100000</f>
+      <c r="G19" s="1">
+        <v>9.5759831300000004E-5</v>
+      </c>
+      <c r="H19">
+        <f>(F19-B19)*100000</f>
         <v>-899806.90000000014</v>
       </c>
-      <c r="F19">
-        <f>(D19-C19)*100000</f>
-        <v>99977.099999999991</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="I19">
+        <f>(F19-D19)*100000</f>
+        <v>-4.900000000007676</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>1</v>
       </c>
       <c r="B20">
         <v>0.59340899999999996</v>
       </c>
+      <c r="C20">
+        <v>1.2E-4</v>
+      </c>
       <c r="D20">
+        <v>0.59277000000000002</v>
+      </c>
+      <c r="E20">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F20">
         <v>0.59225899999999998</v>
       </c>
-      <c r="E20">
-        <f t="shared" ref="E20:E24" si="4">(D20-B20)*100000</f>
+      <c r="G20" s="1">
+        <v>1.3542485199999999E-4</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H24" si="7">(F20-B20)*100000</f>
         <v>-114.99999999999844</v>
       </c>
-      <c r="F20">
-        <f t="shared" ref="F20:F24" si="5">(D20-C20)*100000</f>
-        <v>59225.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="I20">
+        <f t="shared" ref="I20:I24" si="8">(F20-D20)*100000</f>
+        <v>-51.100000000003917</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>2</v>
       </c>
       <c r="D21">
+        <v>0.27517000000000003</v>
+      </c>
+      <c r="E21">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F21">
         <v>0.27416200000000002</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="4"/>
+      <c r="G21" s="1">
+        <v>1.5637515800000001E-4</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
         <v>27416.2</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="5"/>
-        <v>27416.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="I21">
+        <f t="shared" si="8"/>
+        <v>-100.80000000000089</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>3</v>
       </c>
       <c r="B22">
         <v>0.88048999999999999</v>
       </c>
+      <c r="C22" s="1">
+        <v>8.7000000000000001E-5</v>
+      </c>
       <c r="D22">
+        <v>0.88088</v>
+      </c>
+      <c r="E22">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="F22">
         <v>0.87572799999999995</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="4"/>
+      <c r="G22" s="1">
+        <v>9.5759831300000004E-5</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="7"/>
         <v>-476.20000000000442</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="5"/>
-        <v>87572.799999999988</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="I22">
+        <f t="shared" si="8"/>
+        <v>-515.20000000000459</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="D23">
+        <v>1.1009800000000001</v>
+      </c>
+      <c r="E23">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F23">
         <v>1.0971089999999999</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="4"/>
+      <c r="G23" s="1">
+        <v>5.5286964199999999E-5</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="7"/>
         <v>109710.9</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="5"/>
-        <v>109710.9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="I23">
+        <f t="shared" si="8"/>
+        <v>-387.10000000001799</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24">
         <v>1.0757399999999999</v>
       </c>
+      <c r="C24" s="1">
+        <v>7.2000000000000002E-5</v>
+      </c>
       <c r="D24">
+        <v>0.88636000000000004</v>
+      </c>
+      <c r="E24">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="F24">
         <v>1.0738829999999999</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="4"/>
+      <c r="G24" s="1">
+        <v>1.1057392800000001E-4</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="7"/>
         <v>-185.69999999999976</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="5"/>
-        <v>107388.29999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="I24">
+        <f t="shared" si="8"/>
+        <v>18752.299999999988</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="s">
+      <c r="H26" t="s">
         <v>9</v>
       </c>
-      <c r="F26" t="s">
+      <c r="I26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -922,18 +1345,39 @@
         <v>7.24</v>
       </c>
       <c r="D27">
+        <v>30.566666666666599</v>
+      </c>
+      <c r="F27">
         <v>5.24</v>
       </c>
-      <c r="E27">
-        <f>B27/D27</f>
+      <c r="H27">
+        <f>B27/F27</f>
         <v>1.3816793893129771</v>
       </c>
-      <c r="F27">
-        <f>C27/D27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="I27">
+        <f>D27/F27</f>
+        <v>5.8333333333333206</v>
+      </c>
+      <c r="J27">
+        <v>60</v>
+      </c>
+      <c r="K27" s="1">
+        <v>6500000</v>
+      </c>
+      <c r="L27" s="2">
+        <f>J27*K27/(B27*60)</f>
+        <v>897790.05524861871</v>
+      </c>
+      <c r="M27" s="2">
+        <f>J27*K27/(60*D27)</f>
+        <v>212649.94547437344</v>
+      </c>
+      <c r="N27" s="2">
+        <f>J27*K27/(60*F27)</f>
+        <v>1240458.0152671754</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -941,34 +1385,76 @@
         <v>39.409999999999997</v>
       </c>
       <c r="D28">
+        <v>98.4</v>
+      </c>
+      <c r="F28">
         <v>12.26</v>
       </c>
-      <c r="E28">
-        <f t="shared" ref="E28:E32" si="6">B28/D28</f>
+      <c r="H28">
+        <f t="shared" ref="H28:H32" si="9">B28/F28</f>
         <v>3.2145187601957583</v>
       </c>
-      <c r="F28">
-        <f t="shared" ref="F28:F32" si="7">C28/D28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="I28">
+        <f t="shared" ref="I28:I32" si="10">D28/F28</f>
+        <v>8.0261011419249595</v>
+      </c>
+      <c r="J28">
+        <v>60</v>
+      </c>
+      <c r="K28" s="1">
+        <v>6500000</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" ref="L28:L32" si="11">J28*K28/(B28*60)</f>
+        <v>164932.75818320224</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" ref="M28:M32" si="12">J28*K28/(60*D28)</f>
+        <v>66056.91056910569</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" ref="N28:N32" si="13">J28*K28/(60*F28)</f>
+        <v>530179.44535073405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>2</v>
       </c>
       <c r="D29">
+        <v>131.266666666666</v>
+      </c>
+      <c r="F29">
         <v>33.700000000000003</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="6"/>
+      <c r="H29">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="I29">
+        <f t="shared" si="10"/>
+        <v>3.8951533135509195</v>
+      </c>
+      <c r="J29">
+        <v>60</v>
+      </c>
+      <c r="K29" s="1">
+        <v>6500000</v>
+      </c>
+      <c r="L29" s="2" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="12"/>
+        <v>49517.521584560942</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="13"/>
+        <v>192878.33827893174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -976,34 +1462,76 @@
         <v>79.16</v>
       </c>
       <c r="D30">
+        <v>269.46666666666601</v>
+      </c>
+      <c r="F30">
         <v>32.03</v>
       </c>
-      <c r="E30">
-        <f t="shared" si="6"/>
+      <c r="H30">
+        <f t="shared" si="9"/>
         <v>2.4714330315329378</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="I30">
+        <f t="shared" si="10"/>
+        <v>8.4129461962743051</v>
+      </c>
+      <c r="J30">
+        <v>60</v>
+      </c>
+      <c r="K30" s="1">
+        <v>6500000</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="11"/>
+        <v>82112.17786760992</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="12"/>
+        <v>24121.721919841722</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="13"/>
+        <v>202934.74867311894</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>4</v>
       </c>
       <c r="D31">
+        <v>320.39999999999998</v>
+      </c>
+      <c r="F31">
         <v>76.459999999999994</v>
       </c>
-      <c r="E31">
-        <f t="shared" si="6"/>
+      <c r="H31">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="I31">
+        <f t="shared" si="10"/>
+        <v>4.1904263667277011</v>
+      </c>
+      <c r="J31">
+        <v>60</v>
+      </c>
+      <c r="K31" s="1">
+        <v>6000000</v>
+      </c>
+      <c r="L31" s="2" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="12"/>
+        <v>18726.591760299627</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="13"/>
+        <v>78472.403871305272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1011,15 +1539,124 @@
         <v>77.099999999999994</v>
       </c>
       <c r="D32">
+        <v>217.78333333333299</v>
+      </c>
+      <c r="F32">
         <v>42.8</v>
       </c>
-      <c r="E32">
-        <f t="shared" si="6"/>
+      <c r="H32">
+        <f t="shared" si="9"/>
         <v>1.8014018691588785</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="7"/>
-        <v>0</v>
+      <c r="I32">
+        <f t="shared" si="10"/>
+        <v>5.0883956386292759</v>
+      </c>
+      <c r="J32">
+        <v>60</v>
+      </c>
+      <c r="K32" s="1">
+        <v>6500000</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="11"/>
+        <v>84306.095979247737</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="12"/>
+        <v>29846.177393433885</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="13"/>
+        <v>151869.15887850468</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37">
+        <v>9310</v>
+      </c>
+      <c r="I37">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="2">
+        <f>AVERAGE(L10:L15)</f>
+        <v>222843.27316213041</v>
+      </c>
+      <c r="C38" s="2">
+        <f>AVERAGE(M10:M15)</f>
+        <v>75029.199123036597</v>
+      </c>
+      <c r="D38" s="2">
+        <f>AVERAGE(N10:N15)</f>
+        <v>647911.70540021744</v>
+      </c>
+      <c r="G38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38">
+        <v>1321</v>
+      </c>
+      <c r="I38">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="2">
+        <f>B38/H37</f>
+        <v>23.935904743515618</v>
+      </c>
+      <c r="C39" s="2">
+        <f>C38/H37</f>
+        <v>8.0589902387794403</v>
+      </c>
+      <c r="D39" s="2">
+        <f>D38/H38</f>
+        <v>490.47063239986181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="2">
+        <f>B38/I37</f>
+        <v>484.44189817854436</v>
+      </c>
+      <c r="C40" s="2">
+        <f>C38/I37</f>
+        <v>163.10695461529696</v>
+      </c>
+      <c r="D40" s="2">
+        <f>D38/I38</f>
+        <v>2591.6468216008698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assembly reuslts correct now
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -98,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -228,7 +228,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -837,30 +837,30 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1.0757000000000001</v>
+        <v>1.05057</v>
       </c>
       <c r="C7" s="1">
-        <v>6.2000000000000003E-5</v>
+        <v>1.9000000000000001E-4</v>
       </c>
       <c r="D7">
-        <v>0.88634000000000002</v>
-      </c>
-      <c r="E7">
-        <v>4.0000000000000003E-5</v>
+        <v>1.0501199999999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="F7">
-        <v>1.0740259999999999</v>
+        <v>1.0488964300000001</v>
       </c>
       <c r="G7" s="1">
-        <v>7.8187578799999996E-5</v>
+        <v>5.5286964199999999E-5</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>-167.40000000001754</v>
+        <v>-167.35699999999019</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>18768.599999999991</v>
+        <v>-122.35699999998405</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -951,7 +951,7 @@
         <v>9500000</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" ref="L11:N15" si="4">J11*K11/(B11*60)</f>
+        <f t="shared" ref="L11:L15" si="4">J11*K11/(B11*60)</f>
         <v>164246.19640387275</v>
       </c>
       <c r="M11" s="2">
@@ -1088,21 +1088,21 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <v>122.43</v>
+        <v>120.42</v>
       </c>
       <c r="D15">
-        <v>316.45</v>
+        <v>321.27</v>
       </c>
       <c r="F15">
-        <v>41.55</v>
+        <v>43.15</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>2.9465703971119139</v>
+        <v>2.7907300115874856</v>
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>7.6161251504211798</v>
+        <v>7.4454229432213204</v>
       </c>
       <c r="J15">
         <v>60</v>
@@ -1112,15 +1112,15 @@
       </c>
       <c r="L15" s="2">
         <f t="shared" si="4"/>
-        <v>77595.360614228543</v>
+        <v>78890.549742567688</v>
       </c>
       <c r="M15" s="2">
         <f t="shared" si="5"/>
-        <v>30020.540369726656</v>
+        <v>29570.143493012114</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="6"/>
-        <v>228640.1925391095</v>
+        <v>220162.22479721901</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1209,6 +1209,12 @@
       <c r="A21" t="s">
         <v>2</v>
       </c>
+      <c r="B21" s="1">
+        <v>0.27505099999999999</v>
+      </c>
+      <c r="C21">
+        <v>1.8000000000000001E-4</v>
+      </c>
       <c r="D21">
         <v>0.27517000000000003</v>
       </c>
@@ -1223,7 +1229,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="7"/>
-        <v>27416.2</v>
+        <v>-88.89999999999732</v>
       </c>
       <c r="I21">
         <f t="shared" si="8"/>
@@ -1291,30 +1297,30 @@
         <v>5</v>
       </c>
       <c r="B24">
-        <v>1.0757399999999999</v>
+        <v>1.05033</v>
       </c>
       <c r="C24" s="1">
         <v>7.2000000000000002E-5</v>
       </c>
       <c r="D24">
-        <v>0.88636000000000004</v>
+        <v>1.05019</v>
       </c>
       <c r="E24">
-        <v>5.0000000000000002E-5</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="F24">
-        <v>1.0738829999999999</v>
+        <v>1.0488605499999999</v>
       </c>
       <c r="G24" s="1">
-        <v>1.1057392800000001E-4</v>
+        <v>5.5286964199999999E-5</v>
       </c>
       <c r="H24">
         <f t="shared" si="7"/>
-        <v>-185.69999999999976</v>
+        <v>-146.94500000000943</v>
       </c>
       <c r="I24">
         <f t="shared" si="8"/>
-        <v>18752.299999999988</v>
+        <v>-132.94500000000653</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1421,6 +1427,9 @@
       <c r="A29" t="s">
         <v>2</v>
       </c>
+      <c r="B29">
+        <v>146.15</v>
+      </c>
       <c r="D29">
         <v>131.266666666666</v>
       </c>
@@ -1429,7 +1438,7 @@
       </c>
       <c r="H29">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4.3367952522255191</v>
       </c>
       <c r="I29">
         <f t="shared" si="10"/>
@@ -1441,9 +1450,9 @@
       <c r="K29" s="1">
         <v>6500000</v>
       </c>
-      <c r="L29" s="2" t="e">
+      <c r="L29" s="2">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>44474.854601436877</v>
       </c>
       <c r="M29" s="2">
         <f t="shared" si="12"/>
@@ -1535,22 +1544,22 @@
       <c r="A32" t="s">
         <v>5</v>
       </c>
-      <c r="B32">
-        <v>77.099999999999994</v>
+      <c r="B32" s="1">
+        <v>81.537199999999999</v>
       </c>
       <c r="D32">
-        <v>217.78333333333299</v>
+        <v>160.68</v>
       </c>
       <c r="F32">
-        <v>42.8</v>
+        <v>45.06</v>
       </c>
       <c r="H32">
         <f t="shared" si="9"/>
-        <v>1.8014018691588785</v>
+        <v>1.809525077674212</v>
       </c>
       <c r="I32">
         <f t="shared" si="10"/>
-        <v>5.0883956386292759</v>
+        <v>3.5659121171770973</v>
       </c>
       <c r="J32">
         <v>60</v>
@@ -1560,15 +1569,15 @@
       </c>
       <c r="L32" s="2">
         <f t="shared" si="11"/>
-        <v>84306.095979247737</v>
+        <v>79718.214508224468</v>
       </c>
       <c r="M32" s="2">
         <f t="shared" si="12"/>
-        <v>29846.177393433885</v>
+        <v>40453.074433656955</v>
       </c>
       <c r="N32" s="2">
         <f t="shared" si="13"/>
-        <v>151869.15887850468</v>
+        <v>144252.10830004438</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1605,15 +1614,15 @@
       </c>
       <c r="B38" s="2">
         <f>AVERAGE(L10:L15)</f>
-        <v>222843.27316213041</v>
+        <v>223059.1380168536</v>
       </c>
       <c r="C38" s="2">
         <f>AVERAGE(M10:M15)</f>
-        <v>75029.199123036597</v>
+        <v>74954.132976917506</v>
       </c>
       <c r="D38" s="2">
         <f>AVERAGE(N10:N15)</f>
-        <v>647911.70540021744</v>
+        <v>646498.71077656897</v>
       </c>
       <c r="G38" t="s">
         <v>23</v>
@@ -1631,15 +1640,15 @@
       </c>
       <c r="B39" s="2">
         <f>B38/H37</f>
-        <v>23.935904743515618</v>
+        <v>23.959091086665264</v>
       </c>
       <c r="C39" s="2">
         <f>C38/H37</f>
-        <v>8.0589902387794403</v>
+        <v>8.0509272800126208</v>
       </c>
       <c r="D39" s="2">
         <f>D38/H38</f>
-        <v>490.47063239986181</v>
+        <v>489.40099226083947</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1648,15 +1657,15 @@
       </c>
       <c r="B40" s="2">
         <f>B38/I37</f>
-        <v>484.44189817854436</v>
+        <v>484.91116960185565</v>
       </c>
       <c r="C40" s="2">
         <f>C38/I37</f>
-        <v>163.10695461529696</v>
+        <v>162.94376734112501</v>
       </c>
       <c r="D40" s="2">
         <f>D38/I38</f>
-        <v>2591.6468216008698</v>
+        <v>2585.9948431062758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conclusions and future work revisions and combination
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -376,8 +376,8 @@
   </sheetPr>
   <dimension ref="A1:S123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D112" activeCellId="0" sqref="D112"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,7 +521,7 @@
       </c>
       <c r="H3" s="7" t="n">
         <f aca="false">(B3-$D$57)*100000</f>
-        <v>7.24049999999421</v>
+        <v>8.24049999998966</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="8" t="n">
@@ -530,7 +530,7 @@
       </c>
       <c r="K3" s="8" t="n">
         <f aca="false">($D57*$E57+$B3*$C3)*100000</f>
-        <v>9.70879110044179</v>
+        <v>9.70875110044179</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
@@ -545,7 +545,7 @@
       </c>
       <c r="P3" s="8" t="n">
         <f aca="false">($D57*$E57+$B3*$C3)*2*100000</f>
-        <v>19.4175822008836</v>
+        <v>19.4175022008836</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="H20" s="7" t="n">
         <f aca="false">(B20-$D$57)*100000</f>
-        <v>15.387999999994</v>
+        <v>16.3879999999894</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="8" t="n">
@@ -1236,7 +1236,7 @@
       </c>
       <c r="K20" s="8" t="n">
         <f aca="false">($B20*$C20+$D57*$E57)*100000</f>
-        <v>12.2162792271476</v>
+        <v>12.2162392271476</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3" t="s">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="P20" s="8" t="n">
         <f aca="false">($B20*$C20+$D57*$E57)*2*100000</f>
-        <v>24.4325584542953</v>
+        <v>24.4324784542953</v>
       </c>
       <c r="Q20" s="3"/>
       <c r="R20" s="1" t="s">
@@ -1932,7 +1932,7 @@
       </c>
       <c r="H37" s="7" t="n">
         <f aca="false">(B37-$D$57)*100000</f>
-        <v>-7.3447999999976</v>
+        <v>-6.34480000000215</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="8" t="n">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="K37" s="8" t="n">
         <f aca="false">($B37*$C37+$D57*$E57)*100000</f>
-        <v>9.70698798664722</v>
+        <v>9.70694798664722</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3" t="s">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="P37" s="8" t="n">
         <f aca="false">($B37*$C37+$D57*$E57)*2*100000</f>
-        <v>19.4139759732944</v>
+        <v>19.4138959732944</v>
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="1" t="s">
@@ -2622,7 +2622,7 @@
         <v>0.00012</v>
       </c>
       <c r="D57" s="5" t="n">
-        <v>0.5933</v>
+        <v>0.59329</v>
       </c>
       <c r="E57" s="6" t="n">
         <v>4E-005</v>

</xml_diff>